<commit_message>
update UTA , note
</commit_message>
<xml_diff>
--- a/UAT Template.xlsx
+++ b/UAT Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DT1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\UI_PF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E2FFD44C-9CFB-4A3C-894F-06E0937CCD61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3F2E6D-9D57-4535-8B9E-CC497219B03B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UAT Test" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'UAT Test'!$7:$7</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Pass</t>
   </si>
@@ -79,98 +80,122 @@
     <t>APPLICATION 1: หน้า Landing</t>
   </si>
   <si>
-    <t>การกดปุ่มเข้าใช้งาน</t>
-  </si>
-  <si>
     <t>ที่หน้า Landing กดปุ่ม เข้าใช้งาน</t>
   </si>
   <si>
     <t>แสดงหน้าลงชื่อเข้าใช้ระบบ</t>
   </si>
   <si>
-    <t>กดปุ่มสมัครสมาชิก</t>
-  </si>
-  <si>
     <t>ที่หน้า Landing กดปุ่ม สมัครสมาชิก</t>
   </si>
   <si>
     <t>แสดงหน้าสมัครสมาชิก</t>
   </si>
   <si>
-    <t>กดปุ่ม ติดต่อเรา</t>
-  </si>
-  <si>
     <t>ที่หน้า Landing กดปุ่มติดต่อเรา</t>
   </si>
   <si>
     <t>แสดงหน้า ติดต่อเรา</t>
   </si>
   <si>
-    <t>กดปุ่มจัดอันดับ Top 10 ยอดคอมเมนต์สูงสุด และ Top 10 ยอดถูกใจสูงสุด</t>
-  </si>
-  <si>
-    <t>ที่หน้า Landing กดปุ่ม 10กระทู้ยอดคอมเมนต์สูงสุดและปุ่ม 10กระทู้ยอดถูกใจสูงสุด</t>
-  </si>
-  <si>
-    <t>จัดเรียงรายการกระทู้ ตามฟังก์ชันที่กดไว้</t>
-  </si>
-  <si>
-    <t>กดปุ่มเลือกประเภทกระทู้</t>
-  </si>
-  <si>
-    <t>ที่หน้า Landing กดปุ่ม เลือกประเภทกระทู้จากเมนู ประเภทกระทู้ ทางด้านขวามือของหน้า Landing</t>
-  </si>
-  <si>
-    <t>แสดงหน้ารายการกระทู้ตามหัวข้อที่ได้เลือกในเมนู ประเภทเมนู</t>
-  </si>
-  <si>
-    <t>เปิดหน้าจอสมัครสมาชิก จากหน้า ลงชื่อเข้าใช้งาน</t>
-  </si>
-  <si>
-    <t>เปิดหน้าจอสมัครสมาชิกจากหน้า สมัครสมาชิก</t>
-  </si>
-  <si>
-    <t>เปิดหน้าจอสมัครสมาชิกจากหน้า Landing</t>
-  </si>
-  <si>
-    <t>เปิดหน้าจอสมัครสมาชิกจากหน้า คิดต่อเรา</t>
-  </si>
-  <si>
-    <t>เปิดหน้าจอ Landing จากหน้า ลงชื่อเข้าใช้งาน</t>
-  </si>
-  <si>
-    <t>ที่หน้าลงชื่อเข้าใช้งาน กดปุ่มเมนู หน้าหลัก</t>
-  </si>
-  <si>
     <t>แสดงหน้า Landing</t>
   </si>
   <si>
-    <t>เปิดหน้าจอ Landing จากหน้า สมัครสมาชิก</t>
-  </si>
-  <si>
-    <t>ที่หน้าสมัครสมาชิก กดปุ่มเมนู หน้าหลัก</t>
-  </si>
-  <si>
-    <t>เปิดหน้าจอ Landing จากหน้าติดต่อเรา</t>
-  </si>
-  <si>
-    <t>ที่หน้าติดต่อเรา กดปุ่มเมนู หน้าหลัก</t>
-  </si>
-  <si>
-    <t>เปิดหน้าจอ Landing จากหน้าเลือกประเภทกระทู้</t>
-  </si>
-  <si>
-    <t>ที่หน้าประเภทกระทู้ กดปุ่ม หน้าหลัก</t>
-  </si>
-  <si>
     <t>กรอกข้อมูลไม่ครบแบบฟอร์ม</t>
+  </si>
+  <si>
+    <t>กรอกข้อมูลครบถ้วน</t>
+  </si>
+  <si>
+    <t>กรอกข้อมูลลงแบบฟอร์มสมัครสมาชิกครบถ้วนทุกช่อง และ กดยืนยัน CAPTCHA</t>
+  </si>
+  <si>
+    <t>ขึ้น pop up ว่ากรอกข้อมูลไม่ครบ</t>
+  </si>
+  <si>
+    <t>แสดงหน้า ลงชื่อเข้าใช้</t>
+  </si>
+  <si>
+    <t>แสดงหน้า สมัครสมาชิก</t>
+  </si>
+  <si>
+    <t>ไปหน้าจอ ลงชื่อเข้าใช้</t>
+  </si>
+  <si>
+    <t xml:space="preserve">กดที่ปุ่ม ลงชื่อเข้าใช้ </t>
+  </si>
+  <si>
+    <t>ไปหน้า Landing</t>
+  </si>
+  <si>
+    <t>กดที่ปุ่ม หน้าหลัก</t>
+  </si>
+  <si>
+    <t>ไปหน้า ติดต่อเรา</t>
+  </si>
+  <si>
+    <t>กดที่ปุ่ม ติดต่อเรา</t>
+  </si>
+  <si>
+    <t>ไปหน้าสมัครสมาชิก</t>
+  </si>
+  <si>
+    <t>กดที่ปุ่ม สมัครสมาชิก</t>
+  </si>
+  <si>
+    <t>เรียงลำดับกระทู้จาก Top 10 ยอดคอมเมนต์สูงสุด</t>
+  </si>
+  <si>
+    <t>เรียงลำดับกระทู้จาก Top 10 ยอดถูกใจสูงสุด</t>
+  </si>
+  <si>
+    <t>ที่หน้า Landing กดปุ่ม 10กระทู้ยอดคอมเมนต์สูงสุด</t>
+  </si>
+  <si>
+    <t>ที่หน้า Landing กดปุ่ม 10กระทู้ยอดถูกใจสูงสุด</t>
+  </si>
+  <si>
+    <t>แสดง 10 รายการกระทู้โดยเรียงลำดับจาก ยอดคอมเมนต์มากที่สุด10รายการ</t>
+  </si>
+  <si>
+    <t>แสดง 10 รายการกระทู้โดยเรียงลำดับจาก ยอดถูกใจมากที่สุด10รายการ</t>
+  </si>
+  <si>
+    <t>ไปหน้าเข้าใช้งาน</t>
+  </si>
+  <si>
+    <t>ไปติดต่อเรา</t>
+  </si>
+  <si>
+    <t>เลือกดูรายการกระทู้ตามประเภทที่สนใจ</t>
+  </si>
+  <si>
+    <t>ที่หน้า Landing เลือกประเภทกระทู้ จากเมนูทางด้านขวา</t>
+  </si>
+  <si>
+    <t>ไปยังหน้า แสดงรายการกระทู้ตามประเภท</t>
+  </si>
+  <si>
+    <t>แสดง pop up "สมัครสมาชิกสำเร็จ"</t>
+  </si>
+  <si>
+    <t>กรอกข้อมูลไม่ตรงเงื่อนไข</t>
+  </si>
+  <si>
+    <t>แสดง pop up "มีชื่อผู้ใช้นี้ในระบบแล้ว"</t>
+  </si>
+  <si>
+    <t>กรอกข้อมูล ชื่อผู้ใช้ ซ้ำกับ ชื่อผู้ใช้ ที่มีอยู่ในระบบ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ชื้อผู้ใช้งาน : Tester1 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -486,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -508,6 +533,54 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -517,6 +590,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -525,6 +604,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -537,6 +622,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -549,78 +643,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -636,7 +664,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -959,105 +987,105 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V59"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="32.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="32.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="1" customWidth="1"/>
     <col min="6" max="7" width="6" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="11.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="16"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="1:22" ht="59.25" customHeight="1">
+      <c r="A1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:22" ht="18" customHeight="1">
+      <c r="A2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:22" ht="18" customHeight="1">
+      <c r="A3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:22" ht="18" customHeight="1">
+      <c r="A4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="11"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:22" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:22" ht="93.75" customHeight="1">
+      <c r="A5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:22" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+    <row r="6" spans="1:22" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1072,17 +1100,17 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:22" s="10" customFormat="1" ht="15" thickBot="1">
+      <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="9" t="s">
         <v>2</v>
       </c>
@@ -1092,444 +1120,464 @@
       <c r="G7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="30"/>
-    </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="I7" s="37"/>
+    </row>
+    <row r="8" spans="1:22" s="10" customFormat="1" ht="14.4">
+      <c r="A8" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
-    </row>
-    <row r="9" spans="1:22" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+    </row>
+    <row r="9" spans="1:22" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A9" s="13">
         <v>1</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="31" t="s">
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="1:22" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A10" s="13">
+        <v>2</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="40"/>
-    </row>
-    <row r="10" spans="1:22" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35">
+      <c r="D10" s="23"/>
+      <c r="E10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:22" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A11" s="13">
+        <v>3</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:22" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A12" s="13">
+        <v>4</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:22" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A13" s="13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:22" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A14" s="13">
+        <v>6</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:22" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:22" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A17" s="13"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:9" s="6" customFormat="1" ht="64.5" hidden="1" customHeight="1">
+      <c r="A18" s="13">
+        <v>4</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="A19" s="13">
+        <v>5</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+    </row>
+    <row r="21" spans="1:9" s="10" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A21" s="13">
+        <v>1</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="E21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A22" s="13">
         <v>2</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="31" t="s">
+      <c r="B22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A23" s="13">
+        <v>3</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="40"/>
-    </row>
-    <row r="11" spans="1:22" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
-        <v>3</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="36" t="s">
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A24" s="13">
+        <v>4</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="31" t="s">
+      <c r="C24" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A25" s="13">
+        <v>5</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
-    </row>
-    <row r="12" spans="1:22" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
-        <v>4</v>
-      </c>
-      <c r="B12" s="31" t="s">
+      <c r="C25" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="31" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="42"/>
-    </row>
-    <row r="13" spans="1:22" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
-        <v>5</v>
-      </c>
-      <c r="B13" s="31" t="s">
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A26" s="13">
+        <v>6</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A27" s="13">
+        <v>7</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A28" s="13">
+        <v>8</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C28" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-    </row>
-    <row r="14" spans="1:22" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35">
-        <v>6</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="42"/>
-    </row>
-    <row r="15" spans="1:22" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35">
-        <v>7</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
-    </row>
-    <row r="16" spans="1:22" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35">
-        <v>8</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="42"/>
-    </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35">
-        <v>9</v>
-      </c>
-      <c r="B17" s="31" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="42"/>
-    </row>
-    <row r="18" spans="1:9" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="42"/>
-    </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="42"/>
-    </row>
-    <row r="20" spans="1:9" s="6" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="42"/>
-    </row>
-    <row r="21" spans="1:9" s="6" customFormat="1" ht="64.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35">
-        <v>4</v>
-      </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
-    </row>
-    <row r="22" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35">
-        <v>5</v>
-      </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="34"/>
-    </row>
-    <row r="24" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35">
-        <v>1</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="40"/>
-    </row>
-    <row r="25" spans="1:9" s="6" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35">
-        <v>2</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="42"/>
-    </row>
-    <row r="26" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35">
-        <v>3</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="40"/>
-    </row>
-    <row r="27" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35">
-        <v>4</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="42"/>
-    </row>
-    <row r="28" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35">
-        <v>5</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="40"/>
-    </row>
-    <row r="29" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A29" s="13"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A30" s="13"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A31" s="13"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="26"/>
+    </row>
+    <row r="32" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-    </row>
-    <row r="30" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="24"/>
-    </row>
-    <row r="31" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="25"/>
-    </row>
-    <row r="32" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="25"/>
-    </row>
-    <row r="33" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="25"/>
-    </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+    </row>
+    <row r="33" spans="1:9" s="10" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A33" s="8"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="47"/>
+    </row>
+    <row r="34" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A34" s="7"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="25"/>
-    </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="45"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="48"/>
+    </row>
+    <row r="35" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A35" s="7"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="48"/>
+    </row>
+    <row r="36" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A36" s="7"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="48"/>
+    </row>
+    <row r="37" spans="1:9" s="6" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A37" s="7"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="48"/>
+    </row>
+    <row r="38" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1540,7 +1588,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1551,7 +1599,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1562,7 +1610,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1573,7 +1621,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1584,7 +1632,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1595,7 +1643,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1606,7 +1654,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1617,7 +1665,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1628,7 +1676,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1639,7 +1687,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1650,7 +1698,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1661,7 +1709,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1672,7 +1720,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1683,7 +1731,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="2"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1694,7 +1742,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="2"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1705,7 +1753,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="2"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1716,7 +1764,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" s="6" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="2"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1727,7 +1775,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" s="6" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="2"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1738,7 +1786,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" s="6" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A57" s="2"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1749,7 +1797,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" s="6" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" s="6" customFormat="1" ht="65.400000000000006" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1760,7 +1808,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" s="6" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="6" customFormat="1" ht="65.400000000000006" customHeight="1">
       <c r="A59" s="2"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1771,52 +1819,89 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
+    <row r="60" spans="1:9" s="6" customFormat="1" ht="65.400000000000006" customHeight="1">
+      <c r="A60" s="2"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" s="6" customFormat="1" ht="65.400000000000006" customHeight="1">
+      <c r="A61" s="2"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" s="6" customFormat="1" ht="65.400000000000006" customHeight="1">
+      <c r="A62" s="2"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
+  <mergeCells count="48">
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B32:I32"/>
     <mergeCell ref="B33:I33"/>
     <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B37:I37"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H31:I31"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A20:I20"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A32:I32"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H25:I25"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>